<commit_message>
Add v1.0 pin-out pdf.
</commit_message>
<xml_diff>
--- a/ATMega809 Breakout Board - BOM.xlsx
+++ b/ATMega809 Breakout Board - BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Documents\PCB CAD Projects\ATMega809 Breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB5FF97-E80B-4D55-9915-2297B1283F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1FF3D2-132F-408B-9725-77BF04F072A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4932" yWindow="2076" windowWidth="21300" windowHeight="14124" xr2:uid="{B72B0C96-1A16-4432-97CE-7B52F6433A7F}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>1K0</t>
   </si>
   <si>
-    <t xml:space="preserve">1K 0603 resistor; +/-1%; 1/10W </t>
-  </si>
-  <si>
     <t>YAEGO</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>&lt;-- total number of header pins; but only 4 parts (header strips) to place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K0 0603 resistor; +/-1%; 1/10W </t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,31 +714,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -746,13 +746,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -769,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -778,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -795,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -847,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -873,13 +873,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -891,7 +891,7 @@
         <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -899,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -908,7 +908,7 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -925,7 +925,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -951,7 +951,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -960,13 +960,13 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H10">
         <v>3</v>
@@ -977,19 +977,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1000,22 +1000,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
       <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -1026,22 +1026,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1052,22 +1052,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1078,22 +1078,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -1104,22 +1104,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H16">
         <v>3</v>
@@ -1130,22 +1130,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>55</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1156,22 +1156,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>60</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1182,19 +1182,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
         <v>63</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>64</v>
       </c>
-      <c r="F19" t="s">
-        <v>65</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H19">
         <v>1</v>

</xml_diff>